<commit_message>
Fix BE rates 2may18
</commit_message>
<xml_diff>
--- a/required_files/relative risks.xlsx
+++ b/required_files/relative risks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="273840" yWindow="0" windowWidth="21915" windowHeight="11865"/>
+    <workbookView xWindow="276270" yWindow="0" windowWidth="21915" windowHeight="11865"/>
   </bookViews>
   <sheets>
     <sheet name="Use This" sheetId="5" r:id="rId1"/>
@@ -936,8 +936,8 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q32" sqref="Q32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,7 +2846,7 @@
         <v>62</v>
       </c>
       <c r="R39" s="25">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="S39" s="26"/>
     </row>
@@ -2895,7 +2895,9 @@
         <v>9.2543967021286156E-12</v>
       </c>
       <c r="Q40" s="36"/>
-      <c r="R40" s="25"/>
+      <c r="R40" s="25">
+        <v>0.12</v>
+      </c>
       <c r="S40" s="26"/>
     </row>
     <row r="41" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -2947,7 +2949,7 @@
         <v>22</v>
       </c>
       <c r="R41" s="25">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="S41" s="26"/>
     </row>

</xml_diff>

<commit_message>
ann arbor no 2
</commit_message>
<xml_diff>
--- a/required_files/relative risks.xlsx
+++ b/required_files/relative risks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Dropbox\WIP\Risk Prediction\GIT\RiskEA working\IC-RISC-Working\required_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FAA8D3-58A5-4B45-95B6-EEE5B81C3C19}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A3EC85-A7AA-49DD-826F-37ED4B0C8438}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="297945" yWindow="0" windowWidth="21915" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300180" yWindow="0" windowWidth="21915" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use This" sheetId="5" r:id="rId1"/>
@@ -327,11 +327,6 @@
   <si>
     <t>Parasa, S. et al. Gastroenterology 154, 1282-1289.e2 (2018); 
 Sikkema M, et al. Am J Gastro 106, 1231-1238 (2011); Anaparthy, R. et al. ClinGastro Hepatol 11, 1430-1436 (2013)</t>
-  </si>
-  <si>
-    <t>Reid, B. J., Am J Gastroenterol 95, 1669–76 (2000);
-Rastogi, A. et al. Gastrointestinal endoscopy 67, 394–8 (2008); 
-Choi, W.-T. et al. Gut (2017) doi:10.1136/gutjnl-2017-313815; Galipeau, P. C. et al. PLoS medicine 4, e67 (2007).</t>
   </si>
   <si>
     <t>Krishnamoorthi, et al.  Gastro Endo 84, 40–46.e7 (2016);
@@ -473,6 +468,17 @@
       </rPr>
       <t xml:space="preserve"> 9, e103508 (2014)).</t>
     </r>
+  </si>
+  <si>
+    <t>Parasa, Gastroenterology (2018);
+Krishnamoorthi, Am. J. Gastroenterol (2017);
+Duits, Gastroenterology (2017)
+Reid, Am J Gastroenterol 95, 1669–76 (2000);
+Rastogi, Gastrointestinal endoscopy (2008); 
+Choi,  Gut (2017); 
+Galipeau, PLoS medicine 4 (2007);
+Anaparthy, Nature Rev Gastro Hepatology (2014);
+Singh, Gastrointestinal Endoscopy (2014).</t>
   </si>
 </sst>
 </file>
@@ -993,8 +999,8 @@
   <dimension ref="A1:T80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27:H29"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1136,7 @@
         <v>2.08</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="13">
         <v>1</v>
@@ -1194,7 +1200,7 @@
         <v>5.07</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="13">
         <v>2</v>
@@ -1251,7 +1257,7 @@
         <v>7.96</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="13">
         <v>3</v>
@@ -1710,7 +1716,7 @@
         <v>2.76</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
@@ -1791,7 +1797,7 @@
         <v>0.5</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1885,13 +1891,13 @@
       <c r="O17" s="19"/>
       <c r="P17" s="19"/>
       <c r="Q17" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R17" s="61">
         <v>0.25</v>
       </c>
       <c r="S17" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2159,7 +2165,7 @@
     </row>
     <row r="23" spans="1:19" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="21">
         <v>0</v>
@@ -2169,7 +2175,7 @@
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="23">
         <v>0</v>
@@ -2186,18 +2192,18 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="Q23" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R23" s="27">
         <v>1.84E-2</v>
       </c>
       <c r="S23" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="21">
         <v>0</v>
@@ -2209,7 +2215,7 @@
         <v>0.33</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24" s="23">
         <v>1</v>
@@ -2247,7 +2253,7 @@
         <v>0.98160000000000003</v>
       </c>
       <c r="S24" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2303,7 +2309,7 @@
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R26" s="14">
         <v>0.1</v>
@@ -2325,7 +2331,7 @@
         <v>1.6334371714549192</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F27" s="13">
         <v>1</v>
@@ -2382,7 +2388,7 @@
         <v>2.9672581594727543</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F28" s="13">
         <v>2</v>
@@ -2439,7 +2445,7 @@
         <v>4.0143178392147041</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F29" s="13">
         <v>3</v>
@@ -2505,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R30" s="44">
         <v>0.36</v>
@@ -2591,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R32" s="25">
         <v>0.3</v>
@@ -2852,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R37" s="44">
         <v>0.6</v>
@@ -2935,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R39" s="25">
         <v>0.2</v>
@@ -3019,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R41" s="44">
         <v>0.3</v>
@@ -3190,7 +3196,7 @@
       </c>
       <c r="S44" s="45"/>
     </row>
-    <row r="45" spans="1:19" s="24" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="24" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>27</v>
       </c>
@@ -3214,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="Q45" s="36" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="R45" s="25">
         <v>0.85</v>

</xml_diff>